<commit_message>
correcting error in xlsxc file
</commit_message>
<xml_diff>
--- a/contraction_list.xlsx
+++ b/contraction_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinath/Documents/GitHub/cuda_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C212F6C-B9A6-AA42-81BA-1513D06A3602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CAD1D3-2B87-6A49-9F00-0B62178394B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="10460" windowWidth="30240" windowHeight="18880" xr2:uid="{E3220547-C2A3-8B4E-97D6-08DE130750E0}"/>
+    <workbookView xWindow="1860" yWindow="8020" windowWidth="30240" windowHeight="18880" xr2:uid="{E3220547-C2A3-8B4E-97D6-08DE130750E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>adim</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>([-1],[0])</t>
-  </si>
-  <si>
-    <t>floa16</t>
   </si>
   <si>
     <t>ab * cb -&gt; ac-fp16</t>
@@ -462,7 +459,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,10 +531,10 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
         <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -580,10 +577,10 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>